<commit_message>
Finished first draft report
</commit_message>
<xml_diff>
--- a/input/raw_data/final_report/bias_assessment_case_report_end.xlsx
+++ b/input/raw_data/final_report/bias_assessment_case_report_end.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackgedge/Projects/msc_dissertation/iifo_motivation/input/raw_data/final_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B431DC-D022-D94E-9409-03CD108E2040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1818AF18-C21B-B94A-89BF-58C3E507D6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20560" yWindow="880" windowWidth="20580" windowHeight="12240" xr2:uid="{0EC282F7-924A-5B47-8692-5C057716A3B4}"/>
+    <workbookView xWindow="20540" yWindow="880" windowWidth="20580" windowHeight="12240" xr2:uid="{0EC282F7-924A-5B47-8692-5C057716A3B4}"/>
   </bookViews>
   <sheets>
     <sheet name="case_bias_data_start" sheetId="1" r:id="rId1"/>
@@ -1721,8 +1721,8 @@
   <dimension ref="A1:N1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L66" sqref="L66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4627,7 +4627,7 @@
         <v>6</v>
       </c>
       <c r="K66" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="L66" t="s">
         <v>9</v>

</xml_diff>